<commit_message>
address comments from rq3
</commit_message>
<xml_diff>
--- a/resources/averages.xlsx
+++ b/resources/averages.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="22600" tabRatio="500" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="22600" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="whole_word_P_R_F1" sheetId="1" r:id="rId1"/>
@@ -4756,8 +4756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32:I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8628,7 +8628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>

</xml_diff>